<commit_message>
Apenas xlsx, cor no grafico
</commit_message>
<xml_diff>
--- a/media/frases.xlsx
+++ b/media/frases.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73EC9D7-D5C1-4CBA-AA7C-24BF61857839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Bom dia</t>
   </si>
@@ -35,31 +34,14 @@
   </si>
   <si>
     <t>texto</t>
-  </si>
-  <si>
-    <t>No tempo certo, tudo dará certo.</t>
-  </si>
-  <si>
-    <t>Todo dia é dia de alimentar o coração com boas energias.</t>
-  </si>
-  <si>
-    <t>Como esse site é feio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,9 +69,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,16 +350,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -406,26 +387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>